<commit_message>
Actualización de archivos - 25 de junio de 2023 - Lap HP
Se actualiza el repositorio con los archivos que se prepararon para el tercer examen parcial, evaluaciones finales y aclaraciones.
</commit_message>
<xml_diff>
--- a/Calificacion_Examen_Segundo_Parcial.xlsx
+++ b/Calificacion_Examen_Segundo_Parcial.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Fisica 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE029264-B3F9-4E8F-9C1D-43F25A39F4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132230DF-DED6-4212-8926-00336C40A6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{B7EAA70F-132B-4BC7-A44E-B6FF1F284954}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B7EAA70F-132B-4BC7-A44E-B6FF1F284954}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Examen" sheetId="1" r:id="rId1"/>
+    <sheet name="Laboratorio" sheetId="2" r:id="rId2"/>
+    <sheet name="2_Parcial" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2_Parcial'!$B$1:$B$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Laboratorio!$A$1:$E$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="52">
   <si>
     <t>Matrícula</t>
   </si>
@@ -171,12 +177,36 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Práctica 6</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Teoría</t>
+  </si>
+  <si>
+    <t>Faltas</t>
+  </si>
+  <si>
+    <t>Eval_Continua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Puntos_Examen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,8 +243,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -333,11 +369,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -354,13 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -369,13 +410,33 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -770,7 +831,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01665A1A-57AC-47BD-A3BC-473471F01A81}" name="Tabla1" displayName="Tabla1" ref="A1:T22" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01665A1A-57AC-47BD-A3BC-473471F01A81}" name="Tabla1" displayName="Tabla1" ref="A1:T23" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{688F637F-6C63-44C4-BB9D-FB20AA3BDB97}" name="Matrícula" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{8603C639-0D6E-4A64-8EB8-478156C76E5B}" name="Estudiante" dataDxfId="18"/>
@@ -794,7 +855,7 @@
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[P1]:[P15]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="20" xr3:uid="{E0B4A048-47B4-4AF5-A2B8-F6855F59778D}" name="Calificación" dataDxfId="0">
-      <calculatedColumnFormula>Tabla1[[#This Row],[Puntaje]]*0.5</calculatedColumnFormula>
+      <calculatedColumnFormula>(Tabla1[[#This Row],[Puntaje]]*0.66)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1098,20 +1159,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D3C7BB-20D2-4383-A3BC-53B2AF0FEEC2}">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="13"/>
-    <col min="4" max="12" width="5.28515625" style="13" customWidth="1"/>
-    <col min="13" max="18" width="6.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="13"/>
-    <col min="20" max="20" width="13.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="11"/>
+    <col min="4" max="12" width="5.28515625" style="11" customWidth="1"/>
+    <col min="13" max="18" width="6.28515625" style="11" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="11"/>
+    <col min="20" max="20" width="13.28515625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -1183,29 +1244,61 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9">
+        <v>1</v>
+      </c>
+      <c r="N2" s="9">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9">
+        <v>1</v>
+      </c>
+      <c r="P2" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>1</v>
+      </c>
+      <c r="R2" s="9">
+        <v>1</v>
+      </c>
       <c r="S2" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="T2" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1215,29 +1308,61 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
+      <c r="C3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9">
+        <v>1</v>
+      </c>
+      <c r="N3" s="9">
+        <v>1</v>
+      </c>
+      <c r="O3" s="9">
+        <v>1</v>
+      </c>
+      <c r="P3" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>1</v>
+      </c>
+      <c r="R3" s="9">
+        <v>1</v>
+      </c>
       <c r="S3" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="T3" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>8.58</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1247,29 +1372,61 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>1</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0</v>
+      </c>
+      <c r="O4" s="9">
+        <v>1</v>
+      </c>
+      <c r="P4" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>1</v>
+      </c>
+      <c r="R4" s="9">
+        <v>1</v>
+      </c>
       <c r="S4" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="T4" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1279,29 +1436,61 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <v>1</v>
+      </c>
+      <c r="N5" s="9">
+        <v>1</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>1</v>
+      </c>
+      <c r="R5" s="9">
+        <v>1</v>
+      </c>
       <c r="S5" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T5" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>9.5</v>
+      </c>
+      <c r="T5" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.2700000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1311,29 +1500,61 @@
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>1</v>
+      </c>
+      <c r="R6" s="9">
+        <v>1</v>
+      </c>
       <c r="S6" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T6" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="T6" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>7.2600000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1343,29 +1564,61 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+      <c r="M7" s="9">
+        <v>1</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="P7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R7" s="9">
+        <v>0.5</v>
+      </c>
       <c r="S7" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T7" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>8.6</v>
+      </c>
+      <c r="T7" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>5.6760000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1375,29 +1628,61 @@
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9">
+        <v>1</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
+        <v>1</v>
+      </c>
+      <c r="M8" s="9">
+        <v>1</v>
+      </c>
+      <c r="N8" s="9">
+        <v>1</v>
+      </c>
+      <c r="O8" s="9">
+        <v>1</v>
+      </c>
+      <c r="P8" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>0</v>
+      </c>
+      <c r="R8" s="9">
+        <v>1</v>
+      </c>
       <c r="S8" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T8" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="T8" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>7.92</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1407,29 +1692,61 @@
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="9">
+        <v>1</v>
+      </c>
+      <c r="P9" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>1</v>
+      </c>
+      <c r="R9" s="9">
+        <v>1</v>
+      </c>
       <c r="S9" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T9" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="T9" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>7.92</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1439,29 +1756,61 @@
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
+      <c r="M10" s="9">
+        <v>1</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0</v>
+      </c>
+      <c r="O10" s="9">
+        <v>1</v>
+      </c>
+      <c r="P10" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>1</v>
+      </c>
+      <c r="R10" s="9">
+        <v>0</v>
+      </c>
       <c r="S10" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T10" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="T10" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1471,29 +1820,61 @@
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>1</v>
+      </c>
+      <c r="P11" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>1</v>
+      </c>
+      <c r="R11" s="9">
+        <v>1</v>
+      </c>
       <c r="S11" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T11" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="T11" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>5.28</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1503,29 +1884,60 @@
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9">
+        <v>1</v>
+      </c>
+      <c r="M12" s="9">
+        <v>1</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0</v>
+      </c>
+      <c r="O12" s="9">
+        <v>1</v>
+      </c>
+      <c r="P12" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="R12" s="9">
+        <v>0.5</v>
+      </c>
       <c r="S12" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T12" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="T12" s="19">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1535,29 +1947,61 @@
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>1</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>1</v>
+      </c>
+      <c r="O13" s="9">
+        <v>1</v>
+      </c>
+      <c r="P13" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="R13" s="9">
+        <v>0.8</v>
+      </c>
       <c r="S13" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T13" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>10.100000000000001</v>
+      </c>
+      <c r="T13" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.6660000000000013</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1567,29 +2011,61 @@
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0</v>
+      </c>
+      <c r="J14" s="9">
+        <v>1</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0</v>
+      </c>
+      <c r="M14" s="9">
+        <v>1</v>
+      </c>
+      <c r="N14" s="9">
+        <v>0</v>
+      </c>
+      <c r="O14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0.5</v>
+      </c>
       <c r="S14" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T14" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>7.5</v>
+      </c>
+      <c r="T14" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>4.95</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1599,29 +2075,61 @@
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0</v>
+      </c>
+      <c r="L15" s="9">
+        <v>1</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
+      <c r="N15" s="9">
+        <v>1</v>
+      </c>
+      <c r="O15" s="9">
+        <v>1</v>
+      </c>
+      <c r="P15" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="R15" s="9">
+        <v>0.5</v>
+      </c>
       <c r="S15" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>6.8</v>
+      </c>
+      <c r="T15" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>4.4880000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1631,29 +2139,61 @@
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <v>1</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>1</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0</v>
+      </c>
+      <c r="M16" s="9">
+        <v>1</v>
+      </c>
+      <c r="N16" s="9">
+        <v>1</v>
+      </c>
+      <c r="O16" s="9">
+        <v>1</v>
+      </c>
+      <c r="P16" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>1</v>
+      </c>
+      <c r="R16" s="9">
+        <v>0.5</v>
+      </c>
       <c r="S16" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T16" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="T16" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -1663,29 +2203,61 @@
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17" s="9">
+        <v>1</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>1</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>1</v>
+      </c>
+      <c r="N17" s="9">
+        <v>1</v>
+      </c>
+      <c r="O17" s="9">
+        <v>1</v>
+      </c>
+      <c r="P17" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>1</v>
+      </c>
+      <c r="R17" s="9">
+        <v>0</v>
+      </c>
       <c r="S17" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T17" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="T17" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>5.94</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -1695,29 +2267,61 @@
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="C18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0</v>
+      </c>
+      <c r="J18" s="9">
+        <v>1</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>1</v>
+      </c>
+      <c r="N18" s="9">
+        <v>1</v>
+      </c>
+      <c r="O18" s="9">
+        <v>1</v>
+      </c>
+      <c r="P18" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0</v>
+      </c>
+      <c r="R18" s="9">
+        <v>1</v>
+      </c>
       <c r="S18" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T18" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="T18" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>5.28</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -1727,29 +2331,61 @@
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>1</v>
+      </c>
+      <c r="M19" s="9">
+        <v>1</v>
+      </c>
+      <c r="N19" s="9">
+        <v>1</v>
+      </c>
+      <c r="O19" s="9">
+        <v>1</v>
+      </c>
+      <c r="P19" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>1</v>
+      </c>
+      <c r="R19" s="9">
+        <v>1</v>
+      </c>
       <c r="S19" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T19" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="T19" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -1759,29 +2395,61 @@
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1</v>
+      </c>
+      <c r="J20" s="9">
+        <v>1</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0</v>
+      </c>
+      <c r="L20" s="9">
+        <v>0</v>
+      </c>
+      <c r="M20" s="9">
+        <v>1</v>
+      </c>
+      <c r="N20" s="9">
+        <v>1</v>
+      </c>
+      <c r="O20" s="9">
+        <v>1</v>
+      </c>
+      <c r="P20" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>0</v>
+      </c>
+      <c r="R20" s="9">
+        <v>1</v>
+      </c>
       <c r="S20" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T20" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="T20" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>5.94</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -1791,29 +2459,61 @@
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9">
+        <v>1</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21" s="9">
+        <v>1</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+      <c r="N21" s="9">
+        <v>1</v>
+      </c>
+      <c r="O21" s="9">
+        <v>1</v>
+      </c>
+      <c r="P21" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>1</v>
+      </c>
+      <c r="R21" s="9">
+        <v>1</v>
+      </c>
       <c r="S21" s="9">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T21" s="10">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="T21" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -1823,28 +2523,88 @@
       <c r="B22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11">
+      <c r="C22" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1</v>
+      </c>
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0</v>
+      </c>
+      <c r="K22" s="10">
+        <v>0</v>
+      </c>
+      <c r="L22" s="10">
+        <v>1</v>
+      </c>
+      <c r="M22" s="10">
+        <v>1</v>
+      </c>
+      <c r="N22" s="10">
+        <v>1</v>
+      </c>
+      <c r="O22" s="10">
+        <v>1</v>
+      </c>
+      <c r="P22" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>1</v>
+      </c>
+      <c r="R22" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="S22" s="10">
         <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
-        <v>0</v>
-      </c>
-      <c r="T22" s="12">
-        <f>Tabla1[[#This Row],[Puntaje]]*0.5</f>
+        <v>9.5</v>
+      </c>
+      <c r="T22" s="19">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
+        <v>6.2700000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10">
+        <f>SUM(Tabla1[[#This Row],[P1]:[P15]])</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="20">
+        <f>(Tabla1[[#This Row],[Puntaje]]*0.66)</f>
         <v>0</v>
       </c>
     </row>
@@ -1852,49 +2612,49 @@
       <c r="C25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="14" t="s">
+      <c r="N25" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="O25" s="14" t="s">
+      <c r="O25" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="P25" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="Q25" s="14" t="s">
+      <c r="Q25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="R25" s="14" t="s">
+      <c r="R25" s="12" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2018,6 +2778,11 @@
       <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
     </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2025,4 +2790,1081 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8B52A2-B592-40B0-8D3B-0160EE1C6BB7}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>20244190</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13">
+        <v>9</v>
+      </c>
+      <c r="E2" s="13">
+        <f>D2*0.3</f>
+        <v>2.6999999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>20205042</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" ref="E3:E22" si="0">D3*0.3</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>20200429</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>7</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>20214133</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>20244930</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
+        <v>7</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>20236318</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>7</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>20178347</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13">
+        <v>8</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>20239656</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>9</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>2.6999999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>20199353</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0</v>
+      </c>
+      <c r="D10" s="13">
+        <v>8</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>20203695</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>8</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>20214974</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0</v>
+      </c>
+      <c r="D12" s="13">
+        <v>8</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>100237952</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>8</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>20210897</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0</v>
+      </c>
+      <c r="D14" s="13">
+        <v>4</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>20209794</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>6.4</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="0"/>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>20239513</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0</v>
+      </c>
+      <c r="D16" s="13">
+        <v>6.4</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="0"/>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>20214057</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>4</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>20200698</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0</v>
+      </c>
+      <c r="D18" s="13">
+        <v>8</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>20201652</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>9</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>2.6999999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>20206953</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0</v>
+      </c>
+      <c r="D20" s="13">
+        <v>7</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20207436</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>8</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>20197337</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="13">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13">
+        <v>7</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3793837B-BDD6-4632-8685-9EED6BBF55F7}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="11"/>
+    <col min="4" max="4" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="11"/>
+    <col min="6" max="6" width="15.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="11"/>
+    <col min="8" max="8" width="11.85546875" style="11" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>20244190</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13">
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="D2" s="18">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13">
+        <v>6.6</v>
+      </c>
+      <c r="F2" s="13">
+        <f t="shared" ref="F2:F9" si="0">E2*0.5</f>
+        <v>3.3</v>
+      </c>
+      <c r="G2" s="18">
+        <f t="shared" ref="G2:G9" si="1">SUM(D2,F2)</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H2" s="18">
+        <f t="shared" ref="H2:H13" si="2">SUM(C2*0.3,SUM(D2,E2*0.5))</f>
+        <v>9.1100000000000012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>20205042</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="D3" s="17">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="G3" s="18">
+        <f t="shared" si="1"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H3" s="18">
+        <f t="shared" si="2"/>
+        <v>10.020000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>20200429</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="D4" s="18">
+        <v>5</v>
+      </c>
+      <c r="E4" s="13">
+        <v>6.6</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="1"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H4" s="18">
+        <f t="shared" si="2"/>
+        <v>8.9300000000000015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>20214133</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="D5" s="17">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9">
+        <v>6.3</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
+        <v>3.15</v>
+      </c>
+      <c r="G5" s="18">
+        <f t="shared" si="1"/>
+        <v>8.15</v>
+      </c>
+      <c r="H5" s="18">
+        <f t="shared" si="2"/>
+        <v>8.870000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>20244930</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="D6" s="18">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13">
+        <v>7.3</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="0"/>
+        <v>3.65</v>
+      </c>
+      <c r="G6" s="18">
+        <f t="shared" si="1"/>
+        <v>8.65</v>
+      </c>
+      <c r="H6" s="18">
+        <f t="shared" si="2"/>
+        <v>9.2800000000000011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>20236318</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D7" s="17">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>5.7</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>2.85</v>
+      </c>
+      <c r="G7" s="18">
+        <f t="shared" si="1"/>
+        <v>7.85</v>
+      </c>
+      <c r="H7" s="18">
+        <f t="shared" si="2"/>
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>20178347</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="13">
+        <v>2.4</v>
+      </c>
+      <c r="D8" s="18">
+        <v>5</v>
+      </c>
+      <c r="E8" s="13">
+        <v>7.9</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>3.95</v>
+      </c>
+      <c r="G8" s="18">
+        <f t="shared" si="1"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="H8" s="18">
+        <f t="shared" si="2"/>
+        <v>9.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>20239656</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="D9" s="17">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>3.95</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="1"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="H9" s="18">
+        <f t="shared" si="2"/>
+        <v>9.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>20199353</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="13">
+        <v>2.4</v>
+      </c>
+      <c r="D10" s="18">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13">
+        <f>6.6</f>
+        <v>6.6</v>
+      </c>
+      <c r="F10" s="13">
+        <f>E10*0.5</f>
+        <v>3.3</v>
+      </c>
+      <c r="G10" s="18">
+        <f>SUM(D10,F10)</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" si="2"/>
+        <v>9.0200000000000014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>20203695</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="D11" s="17">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5.3</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" ref="F11:F21" si="3">E11*0.5</f>
+        <v>2.65</v>
+      </c>
+      <c r="G11" s="18">
+        <f t="shared" ref="G11:G22" si="4">SUM(D11,F11)</f>
+        <v>7.65</v>
+      </c>
+      <c r="H11" s="18">
+        <f t="shared" si="2"/>
+        <v>8.370000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>20214974</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="13">
+        <v>2.4</v>
+      </c>
+      <c r="D12" s="18">
+        <v>5</v>
+      </c>
+      <c r="E12" s="13">
+        <v>6</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H12" s="18">
+        <f t="shared" si="2"/>
+        <v>8.7200000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>100237952</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="D13" s="17">
+        <v>3.8</v>
+      </c>
+      <c r="E13" s="9">
+        <v>6.7</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="3"/>
+        <v>3.35</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="4"/>
+        <v>7.15</v>
+      </c>
+      <c r="H13" s="18">
+        <f t="shared" si="2"/>
+        <v>7.87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>20210897</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="D14" s="18">
+        <v>5</v>
+      </c>
+      <c r="E14" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="4"/>
+        <v>6.25</v>
+      </c>
+      <c r="H14" s="18">
+        <f>SUM(C14*0.3,SUM(D14,E14*0.5))</f>
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>20209794</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1.92</v>
+      </c>
+      <c r="D15" s="17">
+        <v>5</v>
+      </c>
+      <c r="E15" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="3"/>
+        <v>2.25</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="4"/>
+        <v>7.25</v>
+      </c>
+      <c r="H15" s="18">
+        <f t="shared" ref="H15:H22" si="5">SUM(C15*0.3,SUM(D15,E15*0.5))</f>
+        <v>7.8259999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>20239513</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1.92</v>
+      </c>
+      <c r="D16" s="18">
+        <v>5</v>
+      </c>
+      <c r="E16" s="13">
+        <v>6.6</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="3"/>
+        <v>3.3</v>
+      </c>
+      <c r="G16" s="18">
+        <f t="shared" si="4"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H16" s="18">
+        <f t="shared" si="5"/>
+        <v>8.8760000000000012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>20214057</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="D17" s="17">
+        <v>5</v>
+      </c>
+      <c r="E17" s="9">
+        <v>5.9</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="3"/>
+        <v>2.95</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="4"/>
+        <v>7.95</v>
+      </c>
+      <c r="H17" s="18">
+        <f t="shared" si="5"/>
+        <v>8.31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>20200698</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="13">
+        <v>2.4</v>
+      </c>
+      <c r="D18" s="18">
+        <v>5</v>
+      </c>
+      <c r="E18" s="13">
+        <v>5.3</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="3"/>
+        <v>2.65</v>
+      </c>
+      <c r="G18" s="18">
+        <f t="shared" si="4"/>
+        <v>7.65</v>
+      </c>
+      <c r="H18" s="18">
+        <f t="shared" si="5"/>
+        <v>8.370000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>20201652</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="D19" s="17">
+        <v>5</v>
+      </c>
+      <c r="E19" s="9">
+        <v>6.6</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="3"/>
+        <v>3.3</v>
+      </c>
+      <c r="G19" s="18">
+        <f t="shared" si="4"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H19" s="18">
+        <f t="shared" si="5"/>
+        <v>9.1100000000000012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>20206953</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="D20" s="18">
+        <v>5</v>
+      </c>
+      <c r="E20" s="13">
+        <v>5.9</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="3"/>
+        <v>2.95</v>
+      </c>
+      <c r="G20" s="18">
+        <f t="shared" si="4"/>
+        <v>7.95</v>
+      </c>
+      <c r="H20" s="18">
+        <f t="shared" si="5"/>
+        <v>8.58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20207436</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="D21" s="17">
+        <v>5</v>
+      </c>
+      <c r="E21" s="9">
+        <v>6.6</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="3"/>
+        <v>3.3</v>
+      </c>
+      <c r="G21" s="18">
+        <f t="shared" si="4"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H21" s="18">
+        <f t="shared" si="5"/>
+        <v>9.0200000000000014</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>20197337</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="D22" s="18">
+        <v>3.75</v>
+      </c>
+      <c r="E22" s="13">
+        <v>6.3</v>
+      </c>
+      <c r="F22" s="13">
+        <f>E22*0.5</f>
+        <v>3.15</v>
+      </c>
+      <c r="G22" s="18">
+        <f t="shared" si="4"/>
+        <v>6.9</v>
+      </c>
+      <c r="H22" s="18">
+        <f t="shared" si="5"/>
+        <v>7.53</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B22" xr:uid="{3793837B-BDD6-4632-8685-9EED6BBF55F7}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>